<commit_message>
Update recording coordinate data.xlsx
</commit_message>
<xml_diff>
--- a/recording coordinate data.xlsx
+++ b/recording coordinate data.xlsx
@@ -1316,7 +1316,7 @@
     <t>high activity in the lower bank and possible visual drive. smaller spikes in upper bank. three or four separate groups of activity. getting HC?</t>
   </si>
   <si>
-    <t>5/13/2024</t>
+    <t>5/13/2025</t>
   </si>
   <si>
     <t>E7_03, day 1</t>
@@ -10819,11 +10819,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="453532078"/>
-        <c:axId val="1481490052"/>
+        <c:axId val="407351584"/>
+        <c:axId val="586927276"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="453532078"/>
+        <c:axId val="407351584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10875,10 +10875,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1481490052"/>
+        <c:crossAx val="586927276"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1481490052"/>
+        <c:axId val="586927276"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2500.0"/>
@@ -10954,7 +10954,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453532078"/>
+        <c:crossAx val="407351584"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -11029,11 +11029,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="367481546"/>
-        <c:axId val="898316382"/>
+        <c:axId val="1154056795"/>
+        <c:axId val="1326602403"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="367481546"/>
+        <c:axId val="1154056795"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11085,10 +11085,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="898316382"/>
+        <c:crossAx val="1326602403"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="898316382"/>
+        <c:axId val="1326602403"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4000.0"/>
@@ -11164,7 +11164,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="367481546"/>
+        <c:crossAx val="1154056795"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -11316,11 +11316,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1013990393"/>
-        <c:axId val="1913374655"/>
+        <c:axId val="1539590629"/>
+        <c:axId val="2009451627"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1013990393"/>
+        <c:axId val="1539590629"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11395,10 +11395,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1913374655"/>
+        <c:crossAx val="2009451627"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1913374655"/>
+        <c:axId val="2009451627"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4001.0"/>
@@ -11474,7 +11474,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1013990393"/>
+        <c:crossAx val="1539590629"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -11597,11 +11597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="794957690"/>
-        <c:axId val="897230245"/>
+        <c:axId val="256953769"/>
+        <c:axId val="657456395"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="794957690"/>
+        <c:axId val="256953769"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-28.0"/>
@@ -11677,12 +11677,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="897230245"/>
+        <c:crossAx val="657456395"/>
         <c:majorUnit val="7.0"/>
         <c:minorUnit val="7.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="897230245"/>
+        <c:axId val="657456395"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4100.0"/>
@@ -11758,7 +11758,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="794957690"/>
+        <c:crossAx val="256953769"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -11864,11 +11864,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1598525586"/>
-        <c:axId val="1440662547"/>
+        <c:axId val="692804942"/>
+        <c:axId val="131585726"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1598525586"/>
+        <c:axId val="692804942"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11920,10 +11920,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440662547"/>
+        <c:crossAx val="131585726"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1440662547"/>
+        <c:axId val="131585726"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11998,7 +11998,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1598525586"/>
+        <c:crossAx val="692804942"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -13248,11 +13248,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="401794859"/>
-        <c:axId val="1634249514"/>
+        <c:axId val="1355711532"/>
+        <c:axId val="880229225"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="401794859"/>
+        <c:axId val="1355711532"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13327,10 +13327,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1634249514"/>
+        <c:crossAx val="880229225"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1634249514"/>
+        <c:axId val="880229225"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13405,7 +13405,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="401794859"/>
+        <c:crossAx val="1355711532"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -13481,11 +13481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1406523123"/>
-        <c:axId val="1679370069"/>
+        <c:axId val="1049392477"/>
+        <c:axId val="1939749532"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1406523123"/>
+        <c:axId val="1049392477"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13560,10 +13560,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1679370069"/>
+        <c:crossAx val="1939749532"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1679370069"/>
+        <c:axId val="1939749532"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13638,7 +13638,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1406523123"/>
+        <c:crossAx val="1049392477"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>